<commit_message>
Fixed a small bug in Knapsack
</commit_message>
<xml_diff>
--- a/CT421 - Assignment1.xlsx
+++ b/CT421 - Assignment1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\College\ArtitficialIntelligence\Ass1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DD502DBD-9EAC-4C4A-B1C5-5866AF186559}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C6A345B-EEF5-48C6-8E07-A032D576958E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="4" xr2:uid="{E8969183-0209-4400-8D26-B16CAA3A5CBC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="3" xr2:uid="{E8969183-0209-4400-8D26-B16CAA3A5CBC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -82,8 +82,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2332,9 +2333,9 @@
             <c:numRef>
               <c:f>Sheet4!$A$2:$A$21</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="20"/>
-                <c:pt idx="0">
+                <c:pt idx="0" formatCode="General">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
@@ -2390,9 +2391,6 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2404,64 +2402,61 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>253</c:v>
+                  <c:v>261</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>337</c:v>
+                  <c:v>261</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>267</c:v>
+                  <c:v>261</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>267</c:v>
+                  <c:v>261</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>267</c:v>
+                  <c:v>261</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>267</c:v>
+                  <c:v>261</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>267</c:v>
+                  <c:v>261</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>267</c:v>
+                  <c:v>261</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>267</c:v>
+                  <c:v>261</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>267</c:v>
+                  <c:v>261</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>267</c:v>
+                  <c:v>261</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>267</c:v>
+                  <c:v>261</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>267</c:v>
+                  <c:v>261</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>267</c:v>
+                  <c:v>261</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>267</c:v>
+                  <c:v>261</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>267</c:v>
+                  <c:v>261</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>267</c:v>
+                  <c:v>261</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>267</c:v>
+                  <c:v>261</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>267</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>267</c:v>
+                  <c:v>261</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2503,9 +2498,9 @@
             <c:numRef>
               <c:f>Sheet4!$A$2:$A$21</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="20"/>
-                <c:pt idx="0">
+                <c:pt idx="0" formatCode="General">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
@@ -2561,9 +2556,6 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2575,64 +2567,61 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>78.8</c:v>
+                  <c:v>115.54</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>111.59</c:v>
+                  <c:v>130.72</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>163.29</c:v>
+                  <c:v>152.21</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>205.17</c:v>
+                  <c:v>161.53</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>210.45</c:v>
+                  <c:v>215.06</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>245.21</c:v>
+                  <c:v>250.9</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>253.46</c:v>
+                  <c:v>242.65</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>249.48</c:v>
+                  <c:v>237.25</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>253.22</c:v>
+                  <c:v>248.14</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>249.13</c:v>
+                  <c:v>241.28</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>250.23</c:v>
+                  <c:v>239.26</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>249.81</c:v>
+                  <c:v>243.29</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>251.94</c:v>
+                  <c:v>238.29</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>249.54</c:v>
+                  <c:v>246.07</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>254.39</c:v>
+                  <c:v>241.51</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>248.04</c:v>
+                  <c:v>239.62</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>250.67</c:v>
+                  <c:v>247.86</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>252.41</c:v>
+                  <c:v>244.02</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>247.18</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>242.66</c:v>
+                  <c:v>244.65</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7716,8 +7705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D93C77F5-84DD-48FA-B3F5-5B2D02D101C3}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7743,220 +7732,212 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>253</v>
+        <v>261</v>
       </c>
       <c r="C2">
-        <v>78.8</v>
+        <v>115.54</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>337</v>
+        <v>261</v>
       </c>
       <c r="C3">
-        <v>111.59</v>
+        <v>130.72</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C4">
-        <v>163.29</v>
+        <v>152.21</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C5">
-        <v>205.17</v>
+        <v>161.53</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C6">
-        <v>210.45</v>
+        <v>215.06</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C7">
-        <v>245.21</v>
+        <v>250.9</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C8">
-        <v>253.46</v>
+        <v>242.65</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C9">
-        <v>249.48</v>
+        <v>237.25</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C10">
-        <v>253.22</v>
+        <v>248.14</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C11">
-        <v>249.13</v>
+        <v>241.28</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C12">
-        <v>250.23</v>
+        <v>239.26</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C13">
-        <v>249.81</v>
+        <v>243.29</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C14">
-        <v>251.94</v>
+        <v>238.29</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C15">
-        <v>249.54</v>
+        <v>246.07</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C16">
-        <v>254.39</v>
+        <v>241.51</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C17">
-        <v>248.04</v>
+        <v>239.62</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C18">
-        <v>250.67</v>
+        <v>247.86</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C19">
-        <v>252.41</v>
+        <v>244.02</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C20">
-        <v>247.18</v>
+        <v>244.65</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>19</v>
-      </c>
-      <c r="B21">
-        <v>267</v>
-      </c>
-      <c r="C21">
-        <v>242.66</v>
-      </c>
+      <c r="A21" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7968,7 +7949,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D42EC8E-8682-4A54-96E2-6598C5A41C91}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>

</xml_diff>